<commit_message>
Half Working PWM Out
</commit_message>
<xml_diff>
--- a/Extra/Timesheet.xlsx
+++ b/Extra/Timesheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wede\Documents\GitHub\Plexim_2k18\Extra\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{516B66F0-FBB8-409A-825E-CF0CEA6C979D}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB5955D2-CE3F-47BF-9677-114B505998B9}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -578,8 +578,8 @@
   </sheetPr>
   <dimension ref="A1:H105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="H38" sqref="H38"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="H42" sqref="H42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1195,20 +1195,20 @@
         <v>43300</v>
       </c>
       <c r="C42" s="2">
-        <v>0</v>
+        <v>0.29305555555555557</v>
       </c>
       <c r="D42" s="2">
-        <v>0</v>
+        <v>0.51041666666666663</v>
       </c>
       <c r="E42" s="2">
-        <v>0</v>
+        <v>0.54861111111111105</v>
       </c>
       <c r="F42" s="2">
-        <v>0</v>
+        <v>0.61111111111111105</v>
       </c>
       <c r="G42" s="3">
         <f>(D42-C42)+(F42-E42)</f>
-        <v>0</v>
+        <v>0.27986111111111106</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1244,7 +1244,7 @@
       </c>
       <c r="G45" s="8">
         <f>SUM(G39:G43)</f>
-        <v>0.65138888888888902</v>
+        <v>0.93125000000000013</v>
       </c>
     </row>
     <row r="46" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Mostly done with pwm_out Block
</commit_message>
<xml_diff>
--- a/Extra/Timesheet.xlsx
+++ b/Extra/Timesheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wede\Documents\GitHub\Plexim_2k18\Extra\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB5955D2-CE3F-47BF-9677-114B505998B9}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FED1EE3C-C474-4FFF-844C-0DFC89F53154}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="179017"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -578,8 +579,8 @@
   </sheetPr>
   <dimension ref="A1:H105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="H42" sqref="H42"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="H59" sqref="H59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1221,7 +1222,7 @@
         <v>43301</v>
       </c>
       <c r="C43" s="2">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="D43" s="2">
         <v>0</v>
@@ -1230,11 +1231,11 @@
         <v>0</v>
       </c>
       <c r="F43" s="2">
-        <v>0</v>
+        <v>0.54375000000000007</v>
       </c>
       <c r="G43" s="3">
         <f>(D43-C43)+(F43-E43)</f>
-        <v>0</v>
+        <v>0.24375000000000008</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2"/>
@@ -1244,7 +1245,7 @@
       </c>
       <c r="G45" s="8">
         <f>SUM(G39:G43)</f>
-        <v>0.93125000000000013</v>
+        <v>1.1750000000000003</v>
       </c>
     </row>
     <row r="46" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1279,7 +1280,7 @@
         <v>43304</v>
       </c>
       <c r="C51" s="2">
-        <v>0</v>
+        <v>0.25347222222222221</v>
       </c>
       <c r="D51" s="2">
         <v>0</v>
@@ -1288,11 +1289,11 @@
         <v>0</v>
       </c>
       <c r="F51" s="2">
-        <v>0</v>
+        <v>0.61111111111111105</v>
       </c>
       <c r="G51" s="3">
         <f>(D51-C51)+(F51-E51)</f>
-        <v>0</v>
+        <v>0.35763888888888884</v>
       </c>
     </row>
     <row r="52" spans="1:8" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1406,11 +1407,11 @@
       </c>
       <c r="G57" s="8">
         <f>SUM(G51:G55)</f>
-        <v>0</v>
+        <v>0.35763888888888884</v>
       </c>
       <c r="H57" s="11">
-        <f>SUM(G46, G57)</f>
-        <v>0</v>
+        <f>SUM(G45, G57)</f>
+        <v>1.5326388888888891</v>
       </c>
     </row>
     <row r="60" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
PWM Block Code Complete
</commit_message>
<xml_diff>
--- a/Extra/Timesheet.xlsx
+++ b/Extra/Timesheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wede\Documents\GitHub\Plexim_2k18\Extra\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FED1EE3C-C474-4FFF-844C-0DFC89F53154}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3CF05BF-4D2A-409B-9030-AA08180728D3}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="179017"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -580,7 +579,7 @@
   <dimension ref="A1:H105"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="H59" sqref="H59"/>
+      <selection activeCell="F52" sqref="F52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1283,17 +1282,17 @@
         <v>0.25347222222222221</v>
       </c>
       <c r="D51" s="2">
-        <v>0</v>
+        <v>0.51458333333333328</v>
       </c>
       <c r="E51" s="2">
-        <v>0</v>
+        <v>0.53819444444444442</v>
       </c>
       <c r="F51" s="2">
-        <v>0.61111111111111105</v>
+        <v>0.61458333333333337</v>
       </c>
       <c r="G51" s="3">
         <f>(D51-C51)+(F51-E51)</f>
-        <v>0.35763888888888884</v>
+        <v>0.33750000000000002</v>
       </c>
     </row>
     <row r="52" spans="1:8" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1407,11 +1406,11 @@
       </c>
       <c r="G57" s="8">
         <f>SUM(G51:G55)</f>
-        <v>0.35763888888888884</v>
+        <v>0.33750000000000002</v>
       </c>
       <c r="H57" s="11">
         <f>SUM(G45, G57)</f>
-        <v>1.5326388888888891</v>
+        <v>1.5125000000000002</v>
       </c>
     </row>
     <row r="60" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Plecs "protected table" problem
</commit_message>
<xml_diff>
--- a/Extra/Timesheet.xlsx
+++ b/Extra/Timesheet.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wede\Documents\GitHub\Plexim_2k18\Extra\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wede\Documents\GitHub\OLD\Plexim_2k18\Extra\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAFC7642-DF72-4FFB-8C3E-753E85191387}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BD21CD1-5A20-4C2E-87D2-2A0192FDB3E5}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -578,8 +578,8 @@
   </sheetPr>
   <dimension ref="A1:H105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="H55" sqref="H55"/>
+    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="G61" sqref="G61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1331,20 +1331,20 @@
         <v>43306</v>
       </c>
       <c r="C53" s="2">
-        <v>0</v>
+        <v>0.26250000000000001</v>
       </c>
       <c r="D53" s="2">
-        <v>0</v>
+        <v>0.50555555555555554</v>
       </c>
       <c r="E53" s="2">
-        <v>0</v>
+        <v>0.52986111111111112</v>
       </c>
       <c r="F53" s="2">
-        <v>0</v>
+        <v>0.67013888888888884</v>
       </c>
       <c r="G53" s="3">
         <f>(D53-C53)+(F53-E53)</f>
-        <v>0</v>
+        <v>0.38333333333333325</v>
       </c>
     </row>
     <row r="54" spans="1:8" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1357,20 +1357,20 @@
         <v>43307</v>
       </c>
       <c r="C54" s="2">
-        <v>0</v>
+        <v>0.28333333333333333</v>
       </c>
       <c r="D54" s="2">
-        <v>0</v>
+        <v>0.51527777777777783</v>
       </c>
       <c r="E54" s="2">
-        <v>0</v>
+        <v>0.55347222222222225</v>
       </c>
       <c r="F54" s="2">
-        <v>0</v>
+        <v>0.64583333333333337</v>
       </c>
       <c r="G54" s="3">
         <f>(D54-C54)+(F54-E54)</f>
-        <v>0</v>
+        <v>0.32430555555555562</v>
       </c>
     </row>
     <row r="55" spans="1:8" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1406,11 +1406,11 @@
       </c>
       <c r="G57" s="8">
         <f>SUM(G51:G55)</f>
-        <v>0.62569444444444444</v>
+        <v>1.3333333333333333</v>
       </c>
       <c r="H57" s="11">
         <f>SUM(G45, G57)</f>
-        <v>1.8006944444444448</v>
+        <v>2.5083333333333337</v>
       </c>
     </row>
     <row r="60" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1437,7 +1437,7 @@
         <v>43311</v>
       </c>
       <c r="C63" s="2">
-        <v>0</v>
+        <v>0.28541666666666665</v>
       </c>
       <c r="D63" s="2">
         <v>0</v>
@@ -1446,11 +1446,11 @@
         <v>0</v>
       </c>
       <c r="F63" s="2">
-        <v>0</v>
+        <v>0.61458333333333337</v>
       </c>
       <c r="G63" s="3">
         <f>(D63-C63)+(F63-E63)</f>
-        <v>0</v>
+        <v>0.32916666666666672</v>
       </c>
     </row>
     <row r="64" spans="1:8" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1564,7 +1564,7 @@
       </c>
       <c r="G69" s="8">
         <f>SUM(G63:G67)</f>
-        <v>0</v>
+        <v>0.32916666666666672</v>
       </c>
     </row>
     <row r="72" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Fixed "protected environment" error and errors with make
</commit_message>
<xml_diff>
--- a/Extra/Timesheet.xlsx
+++ b/Extra/Timesheet.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wede\Documents\GitHub\OLD\Plexim_2k18\Extra\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wede\Documents\GitHub\Plexim_2k18\Extra\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BD21CD1-5A20-4C2E-87D2-2A0192FDB3E5}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23F58A2E-9DA9-42E1-A8D6-06EFDFAD7C0A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="18">
   <si>
     <t>Week starting:</t>
   </si>
@@ -78,6 +78,9 @@
   </si>
   <si>
     <t>Week 9/FOOTBALL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
   </si>
 </sst>
 </file>
@@ -578,8 +581,8 @@
   </sheetPr>
   <dimension ref="A1:H105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="G61" sqref="G61"/>
+    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="F65" sqref="F65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1425,6 +1428,9 @@
       <c r="B61" s="7">
         <v>43311</v>
       </c>
+      <c r="G61" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="62" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="63" spans="1:8" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1440,17 +1446,17 @@
         <v>0.28541666666666665</v>
       </c>
       <c r="D63" s="2">
-        <v>0</v>
+        <v>0.49861111111111112</v>
       </c>
       <c r="E63" s="2">
-        <v>0</v>
+        <v>0.51388888888888895</v>
       </c>
       <c r="F63" s="2">
-        <v>0.61458333333333337</v>
+        <v>0.66319444444444442</v>
       </c>
       <c r="G63" s="3">
         <f>(D63-C63)+(F63-E63)</f>
-        <v>0.32916666666666672</v>
+        <v>0.36249999999999993</v>
       </c>
     </row>
     <row r="64" spans="1:8" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1463,7 +1469,7 @@
         <v>43312</v>
       </c>
       <c r="C64" s="2">
-        <v>0</v>
+        <v>0.30208333333333331</v>
       </c>
       <c r="D64" s="2">
         <v>0</v>
@@ -1472,11 +1478,11 @@
         <v>0</v>
       </c>
       <c r="F64" s="2">
-        <v>0</v>
+        <v>0.61458333333333337</v>
       </c>
       <c r="G64" s="3">
         <f>(D64-C64)+(F64-E64)</f>
-        <v>0</v>
+        <v>0.31250000000000006</v>
       </c>
     </row>
     <row r="65" spans="1:7" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1564,7 +1570,7 @@
       </c>
       <c r="G69" s="8">
         <f>SUM(G63:G67)</f>
-        <v>0.32916666666666672</v>
+        <v>0.67500000000000004</v>
       </c>
     </row>
     <row r="72" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>